<commit_message>
Registro de usuarios automatizado
</commit_message>
<xml_diff>
--- a/recursos/DatosLogin.xlsx
+++ b/recursos/DatosLogin.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -602,11 +600,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -618,6 +620,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1">
+        <v>58</v>
+      </c>
       <c r="E1">
         <v>412555441</v>
       </c>
@@ -638,6 +643,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2">
+        <v>33</v>
+      </c>
       <c r="E2">
         <v>412555442</v>
       </c>
@@ -658,6 +666,9 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3">
+        <v>994</v>
+      </c>
       <c r="E3">
         <v>412555443</v>
       </c>
@@ -678,6 +689,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4">
+        <v>994</v>
+      </c>
       <c r="E4">
         <v>412555444</v>
       </c>
@@ -698,6 +712,9 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
+      <c r="D5">
+        <v>1242</v>
+      </c>
       <c r="E5">
         <v>412555445</v>
       </c>
@@ -718,6 +735,9 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="D6">
+        <v>973</v>
+      </c>
       <c r="E6">
         <v>412555446</v>
       </c>
@@ -738,6 +758,9 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
+      <c r="D7">
+        <v>880</v>
+      </c>
       <c r="E7">
         <v>412555447</v>
       </c>
@@ -758,6 +781,9 @@
       <c r="C8" t="s">
         <v>30</v>
       </c>
+      <c r="D8">
+        <v>1246</v>
+      </c>
       <c r="E8">
         <v>412555448</v>
       </c>
@@ -778,6 +804,9 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
+      <c r="D9">
+        <v>375</v>
+      </c>
       <c r="E9">
         <v>412555449</v>
       </c>
@@ -798,6 +827,9 @@
       <c r="C10" t="s">
         <v>38</v>
       </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
       <c r="E10">
         <v>412555450</v>
       </c>
@@ -818,6 +850,9 @@
       <c r="C11" t="s">
         <v>42</v>
       </c>
+      <c r="D11">
+        <v>501</v>
+      </c>
       <c r="E11">
         <v>412555451</v>
       </c>
@@ -838,6 +873,9 @@
       <c r="C12" t="s">
         <v>46</v>
       </c>
+      <c r="D12">
+        <v>229</v>
+      </c>
       <c r="E12">
         <v>412555452</v>
       </c>
@@ -858,6 +896,9 @@
       <c r="C13" t="s">
         <v>50</v>
       </c>
+      <c r="D13">
+        <v>1441</v>
+      </c>
       <c r="E13">
         <v>412555453</v>
       </c>
@@ -878,6 +919,9 @@
       <c r="C14" t="s">
         <v>54</v>
       </c>
+      <c r="D14">
+        <v>975</v>
+      </c>
       <c r="E14">
         <v>412555454</v>
       </c>
@@ -898,6 +942,9 @@
       <c r="C15" t="s">
         <v>58</v>
       </c>
+      <c r="D15">
+        <v>591</v>
+      </c>
       <c r="E15">
         <v>412555455</v>
       </c>
@@ -918,6 +965,9 @@
       <c r="C16" t="s">
         <v>62</v>
       </c>
+      <c r="D16">
+        <v>387</v>
+      </c>
       <c r="E16">
         <v>412555456</v>
       </c>
@@ -938,6 +988,9 @@
       <c r="C17" t="s">
         <v>66</v>
       </c>
+      <c r="D17">
+        <v>267</v>
+      </c>
       <c r="E17">
         <v>412555457</v>
       </c>
@@ -958,6 +1011,9 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
+      <c r="D18">
+        <v>47</v>
+      </c>
       <c r="E18">
         <v>412555458</v>
       </c>
@@ -978,6 +1034,9 @@
       <c r="C19" t="s">
         <v>74</v>
       </c>
+      <c r="D19">
+        <v>55</v>
+      </c>
       <c r="E19">
         <v>412555459</v>
       </c>
@@ -997,6 +1056,9 @@
       </c>
       <c r="C20" t="s">
         <v>78</v>
+      </c>
+      <c r="D20">
+        <v>246</v>
       </c>
       <c r="E20">
         <v>412555460</v>
@@ -1033,28 +1095,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>